<commit_message>
Auto - Update data with bot!
</commit_message>
<xml_diff>
--- a/20210110_old_list_ref.xlsx
+++ b/20210110_old_list_ref.xlsx
@@ -611,12 +611,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>[프로그래머스] 크레인 인형뽑기 게임 in python</t>
+          <t>[프로그래머스] 월간 코드 챌린지 시즌1 &gt; 3진법 뒤집기 in python</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>https://leedakyeong.tistory.com/entry/%ED%94%84%EB%A1%9C%EA%B7%B8%EB%9E%98%EB%A8%B8%EC%8A%A4-%ED%81%AC%EB%A0%88%EC%9D%B8-%EC%9D%B8%ED%98%95%EB%BD%91%EA%B8%B0-%EA%B2%8C%EC%9E%84-in-python</t>
+          <t>https://leedakyeong.tistory.com/entry/%ED%94%84%EB%A1%9C%EA%B7%B8%EB%9E%98%EB%A8%B8%EC%8A%A4-%EC%9B%94%EA%B0%84-%EC%BD%94%EB%93%9C-%EC%B1%8C%EB%A6%B0%EC%A7%80-%EC%8B%9C%EC%A6%8C1-3%EC%A7%84%EB%B2%95-%EB%92%A4%EC%A7%91%EA%B8%B0-in-python</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -707,12 +707,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>L1, L2 정규화에 대한 직관적인 이해</t>
+          <t>데이터 사이언스의 최대 적(敵), 개발자</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://blog.pabii.co.kr/l1-l2-regularization-intuitive-understanding/#utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=l1-l2-regularization-intuitive-understanding</t>
+          <t>https://blog.pabii.co.kr/enemy-data-science-software-engineer/#utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=enemy-data-science-software-engineer</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1155,13 +1155,13 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>"RepVGG: Making VGG-style ConvNets Great Again" 논문 소개
-안녕하세요, Cognex 이호성입니다. 재미있</t>
+          <t>안녕하세요. 평소 머신러닝, 딥러닝에 관심이 많았는데 캐글은 이번에 처음 시작하게 되어 질문 드립니다.
+1. 연구에서도 그렇지만 캐글에서는 특히</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>https://theonly1.tistory.com/2654</t>
+          <t>https://theonly1.tistory.com/2660</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1316,12 +1316,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Point cloud :: numpy를 pcd , pcd를 ply로 바꾸기</t>
+          <t>pytorch로 A3C 구현하면서</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>https://ropiens.tistory.com/71</t>
+          <t>https://ropiens.tistory.com/72</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">

</xml_diff>